<commit_message>
Added the simplified results Emilio wanted for the final display. - This is the base version done for the conversion of the Excel file to r script. The only implementation still needed is to make it dynamic with the UI elements.
</commit_message>
<xml_diff>
--- a/Files/nucleotide_model.xlsx
+++ b/Files/nucleotide_model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\Documents\bpdas\Xext\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909CB7FA-F455-48AA-88F1-29A248D92EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D558565-91FB-4E9C-B46F-E7859613EA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{44207115-4D70-4029-8EC1-48F0BEA38AB7}"/>
   </bookViews>
@@ -1213,7 +1213,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>